<commit_message>
Add further funcionality. Rewrite 'insert_recipe' function.
Added additional fields for prep and cooking times, temperature, and an
allergens list. Rewrote the 'insert_recipe' function to allow for
storing the ingredients list and preparation instructions as arrays.
Added a flash message on submiting the form to indicate success.
Added 'showrecipes.html' to display each recipe and its content.
</commit_message>
<xml_diff>
--- a/design/DB Schema.xlsx
+++ b/design/DB Schema.xlsx
@@ -266,7 +266,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,8 +304,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +343,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -361,13 +373,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,11 +430,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
     <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -703,8 +720,8 @@
   <dimension ref="B1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,7 +852,7 @@
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -871,7 +888,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1005,7 +1022,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1023,7 +1040,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1041,7 +1058,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -1059,7 +1076,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="17" t="s">
         <v>69</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -1077,7 +1094,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -1095,7 +1112,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="6" t="s">

</xml_diff>

<commit_message>
Add testing matrix and update README.md
Added the manual testing matrix for the site and
completed the project README.md file.
</commit_message>
<xml_diff>
--- a/design/DB Schema.xlsx
+++ b/design/DB Schema.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\metal\Code Institute\GitHub\milestone-project-4\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\CI\milestone-project-4\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FBF2B8-9E12-4A4F-B14A-C98263B3E86A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="69">
   <si>
     <t>Collection</t>
   </si>
@@ -138,9 +139,6 @@
   </si>
   <si>
     <t>snack</t>
-  </si>
-  <si>
-    <t>dessert</t>
   </si>
   <si>
     <t>Null/Omit Allowed?</t>
@@ -265,7 +263,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -716,27 +714,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
@@ -753,10 +751,10 @@
         <v>24</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -776,7 +774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -794,10 +792,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -812,7 +810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -830,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -848,7 +846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -868,7 +866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
         <v>31</v>
@@ -886,16 +884,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>1</v>
@@ -904,13 +902,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>13</v>
@@ -922,7 +920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -936,7 +934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -950,7 +948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -964,7 +962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -978,7 +976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -992,7 +990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1006,7 +1004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1020,16 +1018,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>1</v>
@@ -1038,7 +1036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="17" t="s">
         <v>28</v>
@@ -1056,10 +1054,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>29</v>
@@ -1074,10 +1072,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>29</v>
@@ -1092,7 +1090,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="17" t="s">
         <v>30</v>
@@ -1110,13 +1108,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>33</v>
@@ -1128,7 +1126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1142,12 +1140,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>1</v>
@@ -1156,12 +1154,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>1</v>
@@ -1170,12 +1168,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>1</v>
@@ -1184,66 +1182,66 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="16" t="s">
         <v>49</v>
       </c>
+      <c r="F30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="16" t="s">
         <v>50</v>
       </c>
@@ -1254,7 +1252,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1268,7 +1266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1282,7 +1280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1296,7 +1294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1310,7 +1308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1324,7 +1322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1338,7 +1336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1352,7 +1350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1366,7 +1364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1380,7 +1378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1394,7 +1392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1408,7 +1406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1422,7 +1420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1436,7 +1434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1450,7 +1448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1464,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1478,23 +1476,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="E38:E43">
-    <sortCondition ref="E38"/>
+  <sortState ref="E37:E42">
+    <sortCondition ref="E37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>